<commit_message>
--- Auto-Git Commit ---
</commit_message>
<xml_diff>
--- a/DeliveryTemplate.xlsx
+++ b/DeliveryTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\quixx-restart-unmini\03-sep-redesign\Quixx-SPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682FC594-E187-4BF1-9C42-B7CAAD6D5585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6F5B71-DCC4-4F7F-A240-2A79396C0C17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>CUSTOMER</t>
-  </si>
-  <si>
-    <t>Cash on Delivery</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Chocolate</t>
   </si>
@@ -42,33 +36,12 @@
     <t>50</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
     <t>Bring Quixx!</t>
   </si>
   <si>
     <t>Pickup_Time</t>
   </si>
   <si>
-    <t>Delivery_Type</t>
-  </si>
-  <si>
-    <t>Sender_Name</t>
-  </si>
-  <si>
-    <t>Sender_Phone_Number</t>
-  </si>
-  <si>
-    <t>Sender_Address</t>
-  </si>
-  <si>
-    <t>Sender_Lattitude</t>
-  </si>
-  <si>
-    <t>Sender_Longitude</t>
-  </si>
-  <si>
     <t>Receiver_Name</t>
   </si>
   <si>
@@ -81,15 +54,6 @@
     <t>Receiver_Area</t>
   </si>
   <si>
-    <t>Receiver_Lattitude</t>
-  </si>
-  <si>
-    <t>Receiver_Longitude</t>
-  </si>
-  <si>
-    <t>Payment_Method</t>
-  </si>
-  <si>
     <t>Product_Name</t>
   </si>
   <si>
@@ -99,9 +63,6 @@
     <t>Product_Cost</t>
   </si>
   <si>
-    <t>Delivery_Charge</t>
-  </si>
-  <si>
     <t>Delivery_Note</t>
   </si>
   <si>
@@ -111,19 +72,7 @@
     <t>Mirpur Model</t>
   </si>
   <si>
-    <t>Baily Road, Basha-11</t>
-  </si>
-  <si>
-    <t>2: 00 PM</t>
-  </si>
-  <si>
     <t>Ather</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>01971322990</t>
   </si>
   <si>
     <t>01982114988</t>
@@ -133,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,13 +93,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -184,17 +126,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -477,144 +416,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="F1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="22" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" customWidth="1"/>
-    <col min="11" max="11" width="55.140625" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="25.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>